<commit_message>
loader now loads all file endings that I use currently
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Results overview</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>cl50</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>clipp</t>
+  </si>
+  <si>
+    <t>dec</t>
+  </si>
+  <si>
+    <t>e-5</t>
   </si>
 </sst>
 </file>
@@ -408,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +432,7 @@
     <col min="4" max="4" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -436,11 +448,17 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2">
         <v>2</v>
@@ -454,11 +472,17 @@
       <c r="E2" s="2">
         <v>0.24</v>
       </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="2">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2">
         <v>2</v>
@@ -472,11 +496,17 @@
       <c r="E3" s="2">
         <v>0.22</v>
       </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="2">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2">
         <v>4</v>
@@ -490,11 +520,17 @@
       <c r="E4" s="2">
         <v>0.12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>4</v>
       </c>
@@ -504,11 +540,17 @@
       <c r="D5" s="2">
         <v>100</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>5</v>
       </c>
@@ -521,8 +563,14 @@
       <c r="E6" s="2">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -535,8 +583,14 @@
       <c r="E7" s="2">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -549,11 +603,17 @@
       <c r="E8" s="2">
         <v>0.34</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>5</v>
       </c>
@@ -566,11 +626,17 @@
       <c r="E9" s="2">
         <v>0.41</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>5</v>
       </c>
@@ -583,11 +649,17 @@
       <c r="E10" s="2">
         <v>0.31</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>5</v>
       </c>
@@ -600,11 +672,17 @@
       <c r="E11" s="2">
         <v>0.37</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>5</v>
       </c>
@@ -617,11 +695,17 @@
       <c r="E12" s="2">
         <v>0.31</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2">
+        <v>50</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>5</v>
       </c>
@@ -634,8 +718,37 @@
       <c r="E13" s="2">
         <v>0.37</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F14" s="2">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>